<commit_message>
added in cldf writing support
</commit_message>
<xml_diff>
--- a/tests/fixtures/test.xlsx
+++ b/tests/fixtures/test.xlsx
@@ -41,6 +41,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -130,7 +131,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -159,15 +160,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -177,7 +178,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,10 +186,15 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>